<commit_message>
Implemented Strategy pattern for file export.
</commit_message>
<xml_diff>
--- a/LevelMoney/TextFiles/TransactionsData.xlsx
+++ b/LevelMoney/TextFiles/TransactionsData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Transactions" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" r:id="rId1" name="Transactions"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -403,19 +403,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row spans="1:5" outlineLevel="0" r="1">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -432,7 +432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row spans="1:5" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -449,7 +449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row spans="1:5" outlineLevel="0" r="3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -466,7 +466,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row spans="1:5" outlineLevel="0" r="4">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -481,6 +481,31 @@
       </c>
       <c r="E4" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>GMWOGER643</t>
+        </is>
+      </c>
+      <c r="B5" s="1">
+        <v>666</v>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>7.4.2015 г. 00:00:00 ч.</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>IrregularExpense</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>Strategy</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented JSON exporter. Small code fixes
</commit_message>
<xml_diff>
--- a/LevelMoney/TextFiles/TransactionsData.xlsx
+++ b/LevelMoney/TextFiles/TransactionsData.xlsx
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="B6" sqref="B6"/>
@@ -508,6 +508,56 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>DW24LQH232</t>
+        </is>
+      </c>
+      <c r="B6" s="1">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>7.4.2015 г. 00:00:00 ч.</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>IrregularExpense</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>test excel</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>7OFMUXDQU9</t>
+        </is>
+      </c>
+      <c r="B7" s="1">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>7.4.2015 г. 00:00:00 ч.</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>RegularExpense</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
+          <t>2fsd</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added display of expenses per selected date on the main page. The date is exported as short date.
</commit_message>
<xml_diff>
--- a/LevelMoney/TextFiles/TransactionsData.xlsx
+++ b/LevelMoney/TextFiles/TransactionsData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Amount</t>
   </si>
@@ -62,6 +62,27 @@
   </si>
   <si>
     <t>Third</t>
+  </si>
+  <si>
+    <t>GMWOGER643</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>DW24LQH232</t>
+  </si>
+  <si>
+    <t>test excel</t>
+  </si>
+  <si>
+    <t>7OFMUXDQU9</t>
+  </si>
+  <si>
+    <t>2fsd</t>
+  </si>
+  <si>
+    <t>8.4.2015 г. 00:00:00 ч.</t>
   </si>
 </sst>
 </file>
@@ -404,14 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -483,78 +505,104 @@
         <v>15</v>
       </c>
     </row>
-    <row outlineLevel="0" r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>GMWOGER643</t>
-        </is>
+    <row spans="1:5" outlineLevel="0" r="5">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B5" s="1">
         <v>666</v>
       </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>7.4.2015 г. 00:00:00 ч.</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>IrregularExpense</t>
-        </is>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>Strategy</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>DW24LQH232</t>
-        </is>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row spans="1:5" outlineLevel="0" r="6">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B6" s="1">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>7.4.2015 г. 00:00:00 ч.</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="inlineStr">
-        <is>
-          <t>IrregularExpense</t>
-        </is>
-      </c>
-      <c r="E6" s="1" t="inlineStr">
-        <is>
-          <t>test excel</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>7OFMUXDQU9</t>
-        </is>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row spans="1:5" outlineLevel="0" r="7">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B7" s="1">
         <v>34</v>
       </c>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t>7.4.2015 г. 00:00:00 ч.</t>
-        </is>
-      </c>
-      <c r="D7" s="1" t="inlineStr">
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>QCUCJKC37W</t>
+        </is>
+      </c>
+      <c r="B8" s="1">
+        <v>678</v>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>10.4.2015 г. 00:00:00 ч.</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
         <is>
           <t>RegularExpense</t>
         </is>
       </c>
-      <c r="E7" s="1" t="inlineStr">
-        <is>
-          <t>2fsd</t>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>Malko po-dylyg tekst</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>ARKSWRKWDA</t>
+        </is>
+      </c>
+      <c r="B9" s="1">
+        <v>900</v>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>29.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>RegularExpense</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>Muahahaha</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Making the project into two separate projects
Library and Application
</commit_message>
<xml_diff>
--- a/LevelMoney/TextFiles/TransactionsData.xlsx
+++ b/LevelMoney/TextFiles/TransactionsData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Amount</t>
   </si>
@@ -29,60 +29,6 @@
   </si>
   <si>
     <t>Id</t>
-  </si>
-  <si>
-    <t>VDVXC2QEJE</t>
-  </si>
-  <si>
-    <t>1.4.2015 г. 00:00:00 ч.</t>
-  </si>
-  <si>
-    <t>IrregularExpense</t>
-  </si>
-  <si>
-    <t>First Irregular Expense</t>
-  </si>
-  <si>
-    <t>QGZUYP5A74</t>
-  </si>
-  <si>
-    <t>15.4.2015 г. 00:00:00 ч.</t>
-  </si>
-  <si>
-    <t>RegularExpense</t>
-  </si>
-  <si>
-    <t>Second regular exp</t>
-  </si>
-  <si>
-    <t>MZ8LZS4DDI</t>
-  </si>
-  <si>
-    <t>7.4.2015 г. 00:00:00 ч.</t>
-  </si>
-  <si>
-    <t>Third</t>
-  </si>
-  <si>
-    <t>GMWOGER643</t>
-  </si>
-  <si>
-    <t>Strategy</t>
-  </si>
-  <si>
-    <t>DW24LQH232</t>
-  </si>
-  <si>
-    <t>test excel</t>
-  </si>
-  <si>
-    <t>7OFMUXDQU9</t>
-  </si>
-  <si>
-    <t>2fsd</t>
-  </si>
-  <si>
-    <t>8.4.2015 г. 00:00:00 ч.</t>
   </si>
 </sst>
 </file>
@@ -118,9 +64,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -181,7 +126,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -216,7 +161,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -425,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -454,155 +399,30 @@
         <v>3</v>
       </c>
     </row>
-    <row spans="1:5" outlineLevel="0" r="2">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row spans="1:5" outlineLevel="0" r="3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row spans="1:5" outlineLevel="0" r="4">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row spans="1:5" outlineLevel="0" r="5">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1">
-        <v>666</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row spans="1:5" outlineLevel="0" r="6">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row spans="1:5" outlineLevel="0" r="7">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1">
-        <v>34</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="8">
-      <c r="A8" s="1" t="inlineStr">
+    <row outlineLevel="0" r="2">
+      <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>QCUCJKC37W</t>
+          <t>9NTRQ4ECZD</t>
         </is>
       </c>
-      <c r="B8" s="1">
-        <v>678</v>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>10.4.2015 г. 00:00:00 ч.</t>
+          <t>123</t>
         </is>
       </c>
-      <c r="D8" s="1" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>RegularExpense</t>
+          <t>08/04/2015</t>
         </is>
       </c>
-      <c r="E8" s="1" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>Malko po-dylyg tekst</t>
+          <t>RegularIncome</t>
         </is>
       </c>
-    </row>
-    <row outlineLevel="0" r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>ARKSWRKWDA</t>
-        </is>
-      </c>
-      <c r="B9" s="1">
-        <v>900</v>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>29.4.2015 г.</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>RegularExpense</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="inlineStr">
-        <is>
-          <t>Muahahaha</t>
+          <t>IncomeTest</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Making the project into two separate projects"
This reverts commit 19aeea68cc1b61c27248b9703adc720dde7dbf9c.
</commit_message>
<xml_diff>
--- a/LevelMoney/TextFiles/TransactionsData.xlsx
+++ b/LevelMoney/TextFiles/TransactionsData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Amount</t>
   </si>
@@ -29,6 +29,60 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>VDVXC2QEJE</t>
+  </si>
+  <si>
+    <t>1.4.2015 г. 00:00:00 ч.</t>
+  </si>
+  <si>
+    <t>IrregularExpense</t>
+  </si>
+  <si>
+    <t>First Irregular Expense</t>
+  </si>
+  <si>
+    <t>QGZUYP5A74</t>
+  </si>
+  <si>
+    <t>15.4.2015 г. 00:00:00 ч.</t>
+  </si>
+  <si>
+    <t>RegularExpense</t>
+  </si>
+  <si>
+    <t>Second regular exp</t>
+  </si>
+  <si>
+    <t>MZ8LZS4DDI</t>
+  </si>
+  <si>
+    <t>7.4.2015 г. 00:00:00 ч.</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>GMWOGER643</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>DW24LQH232</t>
+  </si>
+  <si>
+    <t>test excel</t>
+  </si>
+  <si>
+    <t>7OFMUXDQU9</t>
+  </si>
+  <si>
+    <t>2fsd</t>
+  </si>
+  <si>
+    <t>8.4.2015 г. 00:00:00 ч.</t>
   </si>
 </sst>
 </file>
@@ -64,8 +118,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -126,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -161,7 +216,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -370,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="A2" sqref="A2:XFD9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -399,30 +454,155 @@
         <v>3</v>
       </c>
     </row>
-    <row outlineLevel="0" r="2">
-      <c r="A2" s="0" t="inlineStr">
-        <is>
-          <t>9NTRQ4ECZD</t>
-        </is>
-      </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>08/04/2015</t>
-        </is>
-      </c>
-      <c r="D2" s="0" t="inlineStr">
-        <is>
-          <t>RegularIncome</t>
-        </is>
-      </c>
-      <c r="E2" s="0" t="inlineStr">
-        <is>
-          <t>IncomeTest</t>
+    <row spans="1:5" outlineLevel="0" r="2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row spans="1:5" outlineLevel="0" r="3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row spans="1:5" outlineLevel="0" r="4">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row spans="1:5" outlineLevel="0" r="5">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>666</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row spans="1:5" outlineLevel="0" r="6">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row spans="1:5" outlineLevel="0" r="7">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>QCUCJKC37W</t>
+        </is>
+      </c>
+      <c r="B8" s="1">
+        <v>678</v>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>10.4.2015 г. 00:00:00 ч.</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>RegularExpense</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>Malko po-dylyg tekst</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>ARKSWRKWDA</t>
+        </is>
+      </c>
+      <c r="B9" s="1">
+        <v>900</v>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>29.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>RegularExpense</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>Muahahaha</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Successfully making it into 2 separate projects
</commit_message>
<xml_diff>
--- a/LevelMoney/TextFiles/TransactionsData.xlsx
+++ b/LevelMoney/TextFiles/TransactionsData.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Transactions"/>
+    <sheet name="Transactions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="true"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Amount</t>
   </si>
@@ -29,60 +29,6 @@
   </si>
   <si>
     <t>Id</t>
-  </si>
-  <si>
-    <t>VDVXC2QEJE</t>
-  </si>
-  <si>
-    <t>1.4.2015 г. 00:00:00 ч.</t>
-  </si>
-  <si>
-    <t>IrregularExpense</t>
-  </si>
-  <si>
-    <t>First Irregular Expense</t>
-  </si>
-  <si>
-    <t>QGZUYP5A74</t>
-  </si>
-  <si>
-    <t>15.4.2015 г. 00:00:00 ч.</t>
-  </si>
-  <si>
-    <t>RegularExpense</t>
-  </si>
-  <si>
-    <t>Second regular exp</t>
-  </si>
-  <si>
-    <t>MZ8LZS4DDI</t>
-  </si>
-  <si>
-    <t>7.4.2015 г. 00:00:00 ч.</t>
-  </si>
-  <si>
-    <t>Third</t>
-  </si>
-  <si>
-    <t>GMWOGER643</t>
-  </si>
-  <si>
-    <t>Strategy</t>
-  </si>
-  <si>
-    <t>DW24LQH232</t>
-  </si>
-  <si>
-    <t>test excel</t>
-  </si>
-  <si>
-    <t>7OFMUXDQU9</t>
-  </si>
-  <si>
-    <t>2fsd</t>
-  </si>
-  <si>
-    <t>8.4.2015 г. 00:00:00 ч.</t>
   </si>
 </sst>
 </file>
@@ -118,9 +64,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -181,7 +126,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -216,7 +161,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -424,20 +369,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:5" outlineLevel="0" r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -454,158 +399,6 @@
         <v>3</v>
       </c>
     </row>
-    <row spans="1:5" outlineLevel="0" r="2">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row spans="1:5" outlineLevel="0" r="3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row spans="1:5" outlineLevel="0" r="4">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row spans="1:5" outlineLevel="0" r="5">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1">
-        <v>666</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row spans="1:5" outlineLevel="0" r="6">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row spans="1:5" outlineLevel="0" r="7">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1">
-        <v>34</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>QCUCJKC37W</t>
-        </is>
-      </c>
-      <c r="B8" s="1">
-        <v>678</v>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>10.4.2015 г. 00:00:00 ч.</t>
-        </is>
-      </c>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>RegularExpense</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="inlineStr">
-        <is>
-          <t>Malko po-dylyg tekst</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>ARKSWRKWDA</t>
-        </is>
-      </c>
-      <c r="B9" s="1">
-        <v>900</v>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>29.4.2015 г.</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>RegularExpense</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="inlineStr">
-        <is>
-          <t>Muahahaha</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding functionality to the Statistics Form
</commit_message>
<xml_diff>
--- a/LevelMoney/TextFiles/TransactionsData.xlsx
+++ b/LevelMoney/TextFiles/TransactionsData.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Transactions" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" r:id="rId1" name="Transactions"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Amount</t>
   </si>
@@ -29,6 +29,27 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>NMRUNEV7JO</t>
+  </si>
+  <si>
+    <t>1233</t>
+  </si>
+  <si>
+    <t>08/04/2015</t>
+  </si>
+  <si>
+    <t>RegularIncome</t>
+  </si>
+  <si>
+    <t>323231</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>9IPFRR6AD1</t>
   </si>
 </sst>
 </file>
@@ -369,20 +390,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row spans="1:5" outlineLevel="0" r="1">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -397,6 +418,229 @@
       </c>
       <c r="E1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row spans="1:5" outlineLevel="0" r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row spans="1:5" outlineLevel="0" r="3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>I43JUZDLPP</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>S5Q1Z1H1Y1</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>45.33</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>asdlkjqaklqwjewe</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>DZO3G7OHMZ</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>44.32</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>IrregularExpense</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>SVEHOIE5BM</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>123.44</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>Salary</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>Q9SPXOVFPD</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>2193.3</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>IrregularIncome</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>Jackpot</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>ZWII13B4U3</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>2213.3</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>IrregularExpense</t>
+        </is>
+      </c>
+      <c r="E9" s="0" t="inlineStr">
+        <is>
+          <t>Robbery</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>CS521O7G9M</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>233.3</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>RegularExpense</t>
+        </is>
+      </c>
+      <c r="E10" s="0" t="inlineStr">
+        <is>
+          <t>MobilePhone</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stats Buttons Functionality added
</commit_message>
<xml_diff>
--- a/LevelMoney/TextFiles/TransactionsData.xlsx
+++ b/LevelMoney/TextFiles/TransactionsData.xlsx
@@ -391,7 +391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="A3" sqref="A3:XFD4"/>
@@ -643,6 +643,60 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>D9ADVKNE1M</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>17/04/2015</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+      <c r="E11" s="0" t="inlineStr">
+        <is>
+          <t>24244</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>AZBGQDJXWI</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>IrregularIncome</t>
+        </is>
+      </c>
+      <c r="E12" s="0" t="inlineStr">
+        <is>
+          <t>1233</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cosmetics added to Statistics form
</commit_message>
<xml_diff>
--- a/LevelMoney/TextFiles/TransactionsData.xlsx
+++ b/LevelMoney/TextFiles/TransactionsData.xlsx
@@ -391,7 +391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="A3" sqref="A3:XFD4"/>
@@ -697,6 +697,249 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>V4XKUQVU51</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>123.484</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+      <c r="E13" s="0" t="inlineStr">
+        <is>
+          <t>12455</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>51E139G34B</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>233.34</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>IrregularExpense</t>
+        </is>
+      </c>
+      <c r="E14" s="0" t="inlineStr">
+        <is>
+          <t>Money</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>2KPOVENKPY</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>1239.4</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>IrregularExpense</t>
+        </is>
+      </c>
+      <c r="E15" s="0" t="inlineStr">
+        <is>
+          <t>Train</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>IPGVVMHLF9</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>12333.4</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>IrregularExpense</t>
+        </is>
+      </c>
+      <c r="E16" s="0" t="inlineStr">
+        <is>
+          <t>Vacation</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>VTY297HZCK</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>234.55</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>IrregularExpense</t>
+        </is>
+      </c>
+      <c r="E17" s="0" t="inlineStr">
+        <is>
+          <t>Hotel</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>7FLBKM7TVW</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>12.55</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>RegularExpense</t>
+        </is>
+      </c>
+      <c r="E18" s="0" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="19">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>WXZWIVXFTG</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>IrregularExpense</t>
+        </is>
+      </c>
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="20">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>1HLZF3HSL1</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="21">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>RHTMK6BYYV</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add exceptions for input validation.
</commit_message>
<xml_diff>
--- a/LevelMoney/TextFiles/TransactionsData.xlsx
+++ b/LevelMoney/TextFiles/TransactionsData.xlsx
@@ -391,7 +391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="A3" sqref="A3:XFD4"/>
@@ -697,6 +697,337 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>OWQ9DY4JY4</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>646</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>8.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>IrregularIncome</t>
+        </is>
+      </c>
+      <c r="E13" s="0" t="inlineStr">
+        <is>
+          <t>дадад</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>77ERLFSCXO</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>6456</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>8.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+      <c r="E14" s="0" t="inlineStr">
+        <is>
+          <t>хжхгхг</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>3F8T2TJK6A</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>-656</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>8.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+      <c r="E15" s="0" t="inlineStr">
+        <is>
+          <t>gfgfgfgfg</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>9112TX7OJP</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>-5454</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>8.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+      <c r="E16" s="0" t="inlineStr">
+        <is>
+          <t>cggfgfg</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>Z9RCKW82NQ</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>654565</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>8.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>IrregularIncome</t>
+        </is>
+      </c>
+      <c r="E17" s="0" t="inlineStr">
+        <is>
+          <t>gfdgfgf</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>CBZQY6LA92</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>8.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>IrregularIncome</t>
+        </is>
+      </c>
+      <c r="E18" s="0" t="inlineStr">
+        <is>
+          <t>gfgfgf</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="19">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>A9UY5NENEM</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>55555</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>8.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>IrregularExpense</t>
+        </is>
+      </c>
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t>tttttttt</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="20">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>LP3949ZN78</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>5656</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>8.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="21">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>8YH22NYVXY</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>64646</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>8.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="22">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>PUXJPLW6XD</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>6565</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>8.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="23">
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>L1XVPLQD2R</t>
+        </is>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>965</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>8.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="24">
+      <c r="A24" s="0" t="inlineStr">
+        <is>
+          <t>5I3AUFJ1EF</t>
+        </is>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>5754</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>8.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>IrregularIncome</t>
+        </is>
+      </c>
+      <c r="E24" s="0" t="inlineStr">
+        <is>
+          <t>hfhh</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="25">
+      <c r="A25" s="0" t="inlineStr">
+        <is>
+          <t>1HI3P6ZLEM</t>
+        </is>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>5464</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>8.4.2015 г.</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>IrregularExpense</t>
+        </is>
+      </c>
+      <c r="E25" s="0" t="inlineStr">
+        <is>
+          <t>хфгхг</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tweaked the Design of StatisticsForm
</commit_message>
<xml_diff>
--- a/LevelMoney/TextFiles/TransactionsData.xlsx
+++ b/LevelMoney/TextFiles/TransactionsData.xlsx
@@ -7,9 +7,9 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Transactions" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" r:id="rId1" name="Transactions"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -369,20 +369,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row spans="1:5" outlineLevel="0" r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -397,6 +397,87 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>9KPTHTAQXE</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>44.5</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>IrregularIncome</t>
+        </is>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t>Eurofootball</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>87VLWB1XEW</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>RegularIncome</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>PayCheck</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>5OVK26GTU5</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>IrregularExpense</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>Lost</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed some button/box names
</commit_message>
<xml_diff>
--- a/LevelMoney/TextFiles/TransactionsData.xlsx
+++ b/LevelMoney/TextFiles/TransactionsData.xlsx
@@ -370,7 +370,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection sqref="A1:E1"/>
@@ -480,6 +480,114 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>GK7CQRV441</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>IrregularIncome</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>Found on the ground</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>RCE8DFA1PV</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>IrregularExpense</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>Robbery</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>DZYM649Q2T</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>RegularExpense</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>TV + INTERNET</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>CUJUW9OMXR</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>3.85</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>08/04/2015</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>IrregularIncome</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>Toto</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>